<commit_message>
Reports import/export feature fully developed!
 — exporting and importing reports done;
— minor code fixes.
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artyom\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D34944-5823-4404-B6A9-F6EDBF564861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA32080A-D769-4CBF-BD6E-94CCC4BCB974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.4"/>
@@ -518,7 +518,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>

</xml_diff>